<commit_message>
xlsxwriter will be replaced with pandas
</commit_message>
<xml_diff>
--- a/reaper.xlsx
+++ b/reaper.xlsx
@@ -7,16 +7,59 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="reapers" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>author</t>
+  </si>
+  <si>
+    <t>creator</t>
+  </si>
+  <si>
+    <t>producer</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>A. Murugan; S.Anu H. Nair; K. P. Sanal Kumar</t>
+  </si>
+  <si>
+    <t>Arbortext Advanced Print Publisher 9.1.440/W Unicode</t>
+  </si>
+  <si>
+    <t>Acrobat Distiller 9.0.0 (Windows); modified using iText® 5.3.5 ©2000-2012 1T3XT BVBA (AGPL-version)</t>
+  </si>
+  <si>
+    <t>J Med Syst, doi:10.1007/s10916-019-1400-8</t>
+  </si>
+  <si>
+    <t>Detection of Skin Cancer Using SVM, Random Forest and kNN Classifiers</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -32,7 +75,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -40,12 +83,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -340,12 +401,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>